<commit_message>
ready for unit test
</commit_message>
<xml_diff>
--- a/test/sample_data_2.xlsx
+++ b/test/sample_data_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joeyc\projects\clara-xlsx-diff\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84613A47-1430-4CE9-BA0C-74490599DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91066CC-CF2C-45E2-B9FE-B13470013ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6350" yWindow="5470" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41740" yWindow="2810" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -607,9 +607,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -649,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -689,7 +689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -709,7 +709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -739,123 +739,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="40.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E6" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:F7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -866,9 +866,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -882,7 +882,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -896,7 +896,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -910,7 +910,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -924,7 +924,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -938,7 +938,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -952,7 +952,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -966,7 +966,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -994,9 +994,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
add example usage command
</commit_message>
<xml_diff>
--- a/test/sample_data_2.xlsx
+++ b/test/sample_data_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joeyc\projects\clara-xlsx-diff\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91066CC-CF2C-45E2-B9FE-B13470013ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468CE18C-FFC9-4846-AE43-8760AD609C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41740" yWindow="2810" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44770" yWindow="3630" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -227,6 +227,27 @@
   </si>
   <si>
     <t>Retention Rate</t>
+  </si>
+  <si>
+    <t>R006</t>
+  </si>
+  <si>
+    <t>R007</t>
+  </si>
+  <si>
+    <t>R008</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>hghhhh</t>
+  </si>
+  <si>
+    <t>lllllll</t>
+  </si>
+  <si>
+    <t>wayyy out here</t>
   </si>
 </sst>
 </file>
@@ -739,10 +760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -750,7 +771,7 @@
     <col min="3" max="3" width="40.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -767,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -784,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -801,7 +822,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>30</v>
       </c>
@@ -818,7 +839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -835,7 +856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -850,6 +871,33 @@
       </c>
       <c r="F7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>